<commit_message>
added asset correlation matrices 2016/2017
</commit_message>
<xml_diff>
--- a/asset_correlation.xlsx
+++ b/asset_correlation.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="14280"/>
   </bookViews>
   <sheets>
-    <sheet name="analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="raw data" sheetId="2" r:id="rId2"/>
+    <sheet name="analysis 2017" sheetId="3" r:id="rId1"/>
+    <sheet name="analysis 2016" sheetId="1" r:id="rId2"/>
+    <sheet name="raw data" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="51">
   <si>
     <t>Asset class correlations for time period 01/01/2016 - 01/31/2017 based on monthly returns.</t>
   </si>
@@ -175,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">PowerShares DB Commodity Tracking </t>
+  </si>
+  <si>
+    <t>Asset class correlations for time period 01/01/2017 - 01/31/2018 based on monthly returns.</t>
   </si>
 </sst>
 </file>
@@ -579,7 +583,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -597,7 +601,7 @@
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>'raw data'!A1</f>
-        <v>Asset class correlations for time period 01/01/2016 - 01/31/2017 based on monthly returns.</v>
+        <v>Asset class correlations for time period 01/01/2017 - 01/31/2018 based on monthly returns.</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
@@ -707,58 +711,58 @@
       </c>
       <c r="D5" s="3">
         <f>'raw data'!D5</f>
-        <v>0.98</v>
+        <v>0.93</v>
       </c>
       <c r="E5" s="3">
         <f>'raw data'!E5</f>
-        <v>0.97</v>
+        <v>0.69</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="3">
         <f>'raw data'!F5</f>
-        <v>-0.5</v>
+        <v>-0.67</v>
       </c>
       <c r="H5" s="3">
         <f>'raw data'!G5</f>
-        <v>-0.22</v>
+        <v>-0.64</v>
       </c>
       <c r="I5" s="3">
         <f>'raw data'!H5</f>
-        <v>-0.35</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="J5" s="3">
         <f>'raw data'!I5</f>
-        <v>-0.17</v>
+        <v>-0.39</v>
       </c>
       <c r="K5" s="3">
         <f>'raw data'!J5</f>
-        <v>-0.23</v>
+        <v>-0.61</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="3">
         <f>'raw data'!K5</f>
-        <v>0.76</v>
+        <v>0.39</v>
       </c>
       <c r="N5" s="3">
         <f>'raw data'!L5</f>
-        <v>0.75</v>
+        <v>0.27</v>
       </c>
       <c r="O5" s="3">
         <f>'raw data'!M5</f>
-        <v>0.6</v>
+        <v>0.36</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="3">
         <f>'raw data'!N5</f>
-        <v>0.66</v>
+        <v>-0.05</v>
       </c>
       <c r="R5" s="3">
         <f>'raw data'!O5</f>
-        <v>0.21</v>
+        <v>0.48</v>
       </c>
       <c r="S5" s="3">
         <f>'raw data'!P5</f>
-        <v>-0.35</v>
+        <v>0.16</v>
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="10" t="s">
@@ -766,15 +770,15 @@
       </c>
       <c r="V5" s="8">
         <f>'raw data'!Q5</f>
-        <v>0.13689999999999999</v>
+        <v>0.25240000000000001</v>
       </c>
       <c r="W5" s="4">
         <f>'raw data'!S5</f>
-        <v>3.15E-2</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="X5" s="4">
         <f>'raw data'!T5</f>
-        <v>0.109</v>
+        <v>5.04E-2</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -786,7 +790,7 @@
       </c>
       <c r="C6" s="3">
         <f>'raw data'!C6</f>
-        <v>0.98</v>
+        <v>0.93</v>
       </c>
       <c r="D6" s="3" t="str">
         <f>'raw data'!D6</f>
@@ -794,54 +798,54 @@
       </c>
       <c r="E6" s="3">
         <f>'raw data'!E6</f>
-        <v>0.96</v>
+        <v>0.71</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="3">
         <f>'raw data'!F6</f>
-        <v>-0.5</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="H6" s="3">
         <f>'raw data'!G6</f>
-        <v>-0.19</v>
+        <v>-0.59</v>
       </c>
       <c r="I6" s="3">
         <f>'raw data'!H6</f>
-        <v>-0.31</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="J6" s="3">
         <f>'raw data'!I6</f>
-        <v>-0.12</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="K6" s="3">
         <f>'raw data'!J6</f>
-        <v>-0.25</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="3">
         <f>'raw data'!K6</f>
-        <v>0.76</v>
+        <v>0.46</v>
       </c>
       <c r="N6" s="3">
         <f>'raw data'!L6</f>
-        <v>0.79</v>
+        <v>0.43</v>
       </c>
       <c r="O6" s="3">
         <f>'raw data'!M6</f>
-        <v>0.63</v>
+        <v>0.34</v>
       </c>
       <c r="P6" s="7"/>
       <c r="Q6" s="3">
         <f>'raw data'!N6</f>
-        <v>0.62</v>
+        <v>0.01</v>
       </c>
       <c r="R6" s="3">
         <f>'raw data'!O6</f>
-        <v>0.18</v>
+        <v>0.37</v>
       </c>
       <c r="S6" s="3">
         <f>'raw data'!P6</f>
-        <v>-0.25</v>
+        <v>0.22</v>
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="12" t="s">
@@ -849,15 +853,15 @@
       </c>
       <c r="V6" s="8">
         <f>'raw data'!Q6</f>
-        <v>0.13350000000000001</v>
+        <v>0.2233</v>
       </c>
       <c r="W6" s="4">
         <f>'raw data'!S6</f>
-        <v>3.7999999999999999E-2</v>
+        <v>1.3899999999999999E-2</v>
       </c>
       <c r="X6" s="4">
         <f>'raw data'!T6</f>
-        <v>0.13170000000000001</v>
+        <v>4.8099999999999997E-2</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -869,11 +873,11 @@
       </c>
       <c r="C7" s="3">
         <f>'raw data'!C7</f>
-        <v>0.97</v>
+        <v>0.69</v>
       </c>
       <c r="D7" s="3">
         <f>'raw data'!D7</f>
-        <v>0.96</v>
+        <v>0.71</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>'raw data'!E7</f>
@@ -882,49 +886,49 @@
       <c r="F7" s="7"/>
       <c r="G7" s="3">
         <f>'raw data'!F7</f>
-        <v>-0.56999999999999995</v>
+        <v>-0.71</v>
       </c>
       <c r="H7" s="3">
         <f>'raw data'!G7</f>
-        <v>-0.31</v>
+        <v>-0.65</v>
       </c>
       <c r="I7" s="3">
         <f>'raw data'!H7</f>
-        <v>-0.42</v>
+        <v>-0.63</v>
       </c>
       <c r="J7" s="3">
         <f>'raw data'!I7</f>
-        <v>-0.27</v>
+        <v>-0.54</v>
       </c>
       <c r="K7" s="3">
         <f>'raw data'!J7</f>
-        <v>-0.37</v>
+        <v>-0.78</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="3">
         <f>'raw data'!K7</f>
-        <v>0.64</v>
+        <v>-0.03</v>
       </c>
       <c r="N7" s="3">
         <f>'raw data'!L7</f>
-        <v>0.65</v>
+        <v>0.02</v>
       </c>
       <c r="O7" s="3">
         <f>'raw data'!M7</f>
-        <v>0.46</v>
+        <v>-0.12</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="3">
         <f>'raw data'!N7</f>
-        <v>0.56000000000000005</v>
+        <v>0.24</v>
       </c>
       <c r="R7" s="3">
         <f>'raw data'!O7</f>
-        <v>0.24</v>
+        <v>0.37</v>
       </c>
       <c r="S7" s="3">
         <f>'raw data'!P7</f>
-        <v>-0.36</v>
+        <v>-0.32</v>
       </c>
       <c r="T7" s="7"/>
       <c r="U7" s="10" t="s">
@@ -932,15 +936,15 @@
       </c>
       <c r="V7" s="8">
         <f>'raw data'!Q7</f>
-        <v>0.18540000000000001</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="W7" s="4">
         <f>'raw data'!S7</f>
-        <v>4.36E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="X7" s="4">
         <f>'raw data'!T7</f>
-        <v>0.15090000000000001</v>
+        <v>5.5199999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -978,15 +982,15 @@
       </c>
       <c r="C9" s="3">
         <f>'raw data'!C8</f>
-        <v>-0.5</v>
+        <v>-0.67</v>
       </c>
       <c r="D9" s="3">
         <f>'raw data'!D8</f>
-        <v>-0.5</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="E9" s="3">
         <f>'raw data'!E8</f>
-        <v>-0.56999999999999995</v>
+        <v>-0.71</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="3" t="str">
@@ -995,45 +999,45 @@
       </c>
       <c r="H9" s="3">
         <f>'raw data'!G8</f>
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="I9" s="3">
         <f>'raw data'!H8</f>
-        <v>0.84</v>
+        <v>0.63</v>
       </c>
       <c r="J9" s="3">
         <f>'raw data'!I8</f>
-        <v>0.87</v>
+        <v>0.7</v>
       </c>
       <c r="K9" s="3">
         <f>'raw data'!J8</f>
-        <v>0.68</v>
+        <v>0.79</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="3">
         <f>'raw data'!K8</f>
-        <v>-0.17</v>
+        <v>-0.09</v>
       </c>
       <c r="N9" s="3">
         <f>'raw data'!L8</f>
-        <v>-0.22</v>
+        <v>0.08</v>
       </c>
       <c r="O9" s="3">
         <f>'raw data'!M8</f>
-        <v>0.13</v>
+        <v>0.05</v>
       </c>
       <c r="P9" s="7"/>
       <c r="Q9" s="3">
         <f>'raw data'!N8</f>
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="R9" s="3">
         <f>'raw data'!O8</f>
-        <v>-0.03</v>
+        <v>-0.38</v>
       </c>
       <c r="S9" s="3">
         <f>'raw data'!P8</f>
-        <v>0.73</v>
+        <v>0.43</v>
       </c>
       <c r="T9" s="7"/>
       <c r="U9" s="10" t="s">
@@ -1041,15 +1045,15 @@
       </c>
       <c r="V9" s="8">
         <f>'raw data'!Q8</f>
-        <v>8.6E-3</v>
+        <v>-2.0000000000000001E-4</v>
       </c>
       <c r="W9" s="4">
         <f>'raw data'!S8</f>
-        <v>3.0000000000000001E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="X9" s="4">
         <f>'raw data'!T8</f>
-        <v>1.04E-2</v>
+        <v>5.5999999999999999E-3</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1061,20 +1065,20 @@
       </c>
       <c r="C10" s="3">
         <f>'raw data'!C9</f>
-        <v>-0.22</v>
+        <v>-0.64</v>
       </c>
       <c r="D10" s="3">
         <f>'raw data'!D9</f>
-        <v>-0.19</v>
+        <v>-0.59</v>
       </c>
       <c r="E10" s="3">
         <f>'raw data'!E9</f>
-        <v>-0.31</v>
+        <v>-0.65</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="3">
         <f>'raw data'!F9</f>
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="H10" s="3" t="str">
         <f>'raw data'!G9</f>
@@ -1082,11 +1086,11 @@
       </c>
       <c r="I10" s="3">
         <f>'raw data'!H9</f>
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="J10" s="3">
         <f>'raw data'!I9</f>
-        <v>0.93</v>
+        <v>0.72</v>
       </c>
       <c r="K10" s="3">
         <f>'raw data'!J9</f>
@@ -1095,15 +1099,15 @@
       <c r="L10" s="7"/>
       <c r="M10" s="3">
         <f>'raw data'!K9</f>
-        <v>0.14000000000000001</v>
+        <v>-0.47</v>
       </c>
       <c r="N10" s="3">
         <f>'raw data'!L9</f>
-        <v>0.14000000000000001</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="O10" s="3">
         <f>'raw data'!M9</f>
-        <v>0.38</v>
+        <v>-0.32</v>
       </c>
       <c r="P10" s="7"/>
       <c r="Q10" s="3">
@@ -1112,11 +1116,11 @@
       </c>
       <c r="R10" s="3">
         <f>'raw data'!O9</f>
-        <v>0.01</v>
+        <v>-0.35</v>
       </c>
       <c r="S10" s="3">
         <f>'raw data'!P9</f>
-        <v>0.77</v>
+        <v>0.26</v>
       </c>
       <c r="T10" s="7"/>
       <c r="U10" s="12" t="s">
@@ -1124,15 +1128,15 @@
       </c>
       <c r="V10" s="8">
         <f>'raw data'!Q9</f>
-        <v>2.5000000000000001E-2</v>
+        <v>2.1100000000000001E-2</v>
       </c>
       <c r="W10" s="4">
         <f>'raw data'!S9</f>
-        <v>1.11E-2</v>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="X10" s="4">
         <f>'raw data'!T9</f>
-        <v>3.8399999999999997E-2</v>
+        <v>2.0299999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1144,24 +1148,24 @@
       </c>
       <c r="C11" s="3">
         <f>'raw data'!C10</f>
-        <v>-0.35</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="D11" s="3">
         <f>'raw data'!D10</f>
-        <v>-0.31</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="E11" s="3">
         <f>'raw data'!E10</f>
-        <v>-0.42</v>
+        <v>-0.63</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="3">
         <f>'raw data'!F10</f>
-        <v>0.84</v>
+        <v>0.63</v>
       </c>
       <c r="H11" s="3">
         <f>'raw data'!G10</f>
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="I11" s="3" t="str">
         <f>'raw data'!H10</f>
@@ -1169,37 +1173,37 @@
       </c>
       <c r="J11" s="3">
         <f>'raw data'!I10</f>
-        <v>0.85</v>
+        <v>0.69</v>
       </c>
       <c r="K11" s="3">
         <f>'raw data'!J10</f>
-        <v>0.78</v>
+        <v>0.69</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="3">
         <f>'raw data'!K10</f>
-        <v>-0.09</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="N11" s="3">
         <f>'raw data'!L10</f>
-        <v>-0.08</v>
+        <v>-0.43</v>
       </c>
       <c r="O11" s="3">
         <f>'raw data'!M10</f>
-        <v>0.16</v>
+        <v>-0.33</v>
       </c>
       <c r="P11" s="7"/>
       <c r="Q11" s="3">
         <f>'raw data'!N10</f>
-        <v>0.36</v>
+        <v>0.48</v>
       </c>
       <c r="R11" s="3">
         <f>'raw data'!O10</f>
-        <v>-0.21</v>
+        <v>-0.38</v>
       </c>
       <c r="S11" s="3">
         <f>'raw data'!P10</f>
-        <v>0.76</v>
+        <v>0.32</v>
       </c>
       <c r="T11" s="7"/>
       <c r="U11" s="10" t="s">
@@ -1207,15 +1211,15 @@
       </c>
       <c r="V11" s="8">
         <f>'raw data'!Q10</f>
-        <v>1.8499999999999999E-2</v>
+        <v>5.1900000000000002E-2</v>
       </c>
       <c r="W11" s="4">
         <f>'raw data'!S10</f>
-        <v>3.9199999999999999E-2</v>
+        <v>1.8200000000000001E-2</v>
       </c>
       <c r="X11" s="4">
         <f>'raw data'!T10</f>
-        <v>0.1358</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1227,28 +1231,28 @@
       </c>
       <c r="C12" s="3">
         <f>'raw data'!C11</f>
-        <v>-0.17</v>
+        <v>-0.39</v>
       </c>
       <c r="D12" s="3">
         <f>'raw data'!D11</f>
-        <v>-0.12</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="E12" s="3">
         <f>'raw data'!E11</f>
-        <v>-0.27</v>
+        <v>-0.54</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="3">
         <f>'raw data'!F11</f>
-        <v>0.87</v>
+        <v>0.7</v>
       </c>
       <c r="H12" s="3">
         <f>'raw data'!G11</f>
-        <v>0.93</v>
+        <v>0.72</v>
       </c>
       <c r="I12" s="3">
         <f>'raw data'!H11</f>
-        <v>0.85</v>
+        <v>0.69</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>'raw data'!I11</f>
@@ -1256,33 +1260,33 @@
       </c>
       <c r="K12" s="3">
         <f>'raw data'!J11</f>
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="3">
         <f>'raw data'!K11</f>
-        <v>0.2</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="N12" s="3">
         <f>'raw data'!L11</f>
-        <v>0.19</v>
+        <v>0.09</v>
       </c>
       <c r="O12" s="3">
         <f>'raw data'!M11</f>
-        <v>0.51</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="P12" s="7"/>
       <c r="Q12" s="3">
         <f>'raw data'!N11</f>
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
       <c r="R12" s="3">
         <f>'raw data'!O11</f>
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="S12" s="3">
         <f>'raw data'!P11</f>
-        <v>0.81</v>
+        <v>0.66</v>
       </c>
       <c r="T12" s="7"/>
       <c r="U12" s="12" t="s">
@@ -1290,15 +1294,15 @@
       </c>
       <c r="V12" s="8">
         <f>'raw data'!Q11</f>
-        <v>5.1700000000000003E-2</v>
+        <v>1.89E-2</v>
       </c>
       <c r="W12" s="4">
         <f>'raw data'!S11</f>
-        <v>1.17E-2</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="X12" s="4">
         <f>'raw data'!T11</f>
-        <v>4.0399999999999998E-2</v>
+        <v>2.24E-2</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1310,20 +1314,20 @@
       </c>
       <c r="C13" s="3">
         <f>'raw data'!C12</f>
-        <v>-0.23</v>
+        <v>-0.61</v>
       </c>
       <c r="D13" s="3">
         <f>'raw data'!D12</f>
-        <v>-0.25</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="E13" s="3">
         <f>'raw data'!E12</f>
-        <v>-0.37</v>
+        <v>-0.78</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="3">
         <f>'raw data'!F12</f>
-        <v>0.68</v>
+        <v>0.79</v>
       </c>
       <c r="H13" s="3">
         <f>'raw data'!G12</f>
@@ -1331,11 +1335,11 @@
       </c>
       <c r="I13" s="3">
         <f>'raw data'!H12</f>
-        <v>0.78</v>
+        <v>0.69</v>
       </c>
       <c r="J13" s="3">
         <f>'raw data'!I12</f>
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="K13" s="3" t="str">
         <f>'raw data'!J12</f>
@@ -1344,28 +1348,28 @@
       <c r="L13" s="7"/>
       <c r="M13" s="3">
         <f>'raw data'!K12</f>
-        <v>0.21</v>
+        <v>-0.13</v>
       </c>
       <c r="N13" s="3">
         <f>'raw data'!L12</f>
-        <v>0.14000000000000001</v>
+        <v>-0.05</v>
       </c>
       <c r="O13" s="3">
         <f>'raw data'!M12</f>
-        <v>0.28000000000000003</v>
+        <v>-0.12</v>
       </c>
       <c r="P13" s="7"/>
       <c r="Q13" s="3">
         <f>'raw data'!N12</f>
-        <v>0.4</v>
+        <v>0.18</v>
       </c>
       <c r="R13" s="3">
         <f>'raw data'!O12</f>
-        <v>0.14000000000000001</v>
+        <v>-0.2</v>
       </c>
       <c r="S13" s="3">
         <f>'raw data'!P12</f>
-        <v>0.54</v>
+        <v>0.24</v>
       </c>
       <c r="T13" s="7"/>
       <c r="U13" s="10" t="s">
@@ -1373,15 +1377,15 @@
       </c>
       <c r="V13" s="8">
         <f>'raw data'!Q12</f>
-        <v>8.9999999999999998E-4</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="W13" s="4">
         <f>'raw data'!S12</f>
-        <v>1.44E-2</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="X13" s="4">
         <f>'raw data'!T12</f>
-        <v>0.05</v>
+        <v>2.5499999999999998E-2</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1419,36 +1423,36 @@
       </c>
       <c r="C15" s="3">
         <f>'raw data'!C13</f>
-        <v>0.76</v>
+        <v>0.39</v>
       </c>
       <c r="D15" s="3">
         <f>'raw data'!D13</f>
-        <v>0.76</v>
+        <v>0.46</v>
       </c>
       <c r="E15" s="3">
         <f>'raw data'!E13</f>
-        <v>0.64</v>
+        <v>-0.03</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="3">
         <f>'raw data'!F13</f>
-        <v>-0.17</v>
+        <v>-0.09</v>
       </c>
       <c r="H15" s="3">
         <f>'raw data'!G13</f>
-        <v>0.14000000000000001</v>
+        <v>-0.47</v>
       </c>
       <c r="I15" s="3">
         <f>'raw data'!H13</f>
-        <v>-0.09</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="J15" s="3">
         <f>'raw data'!I13</f>
-        <v>0.2</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="K15" s="3">
         <f>'raw data'!J13</f>
-        <v>0.21</v>
+        <v>-0.13</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="3" t="str">
@@ -1457,24 +1461,24 @@
       </c>
       <c r="N15" s="3">
         <f>'raw data'!L13</f>
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="O15" s="3">
         <f>'raw data'!M13</f>
-        <v>0.87</v>
+        <v>0.8</v>
       </c>
       <c r="P15" s="7"/>
       <c r="Q15" s="3">
         <f>'raw data'!N13</f>
-        <v>0.6</v>
+        <v>-0.72</v>
       </c>
       <c r="R15" s="3">
         <f>'raw data'!O13</f>
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
       <c r="S15" s="3">
         <f>'raw data'!P13</f>
-        <v>-7.0000000000000007E-2</v>
+        <v>0.36</v>
       </c>
       <c r="T15" s="7"/>
       <c r="U15" s="10" t="s">
@@ -1482,15 +1486,15 @@
       </c>
       <c r="V15" s="8">
         <f>'raw data'!Q13</f>
-        <v>8.5099999999999995E-2</v>
+        <v>0.31669999999999998</v>
       </c>
       <c r="W15" s="4">
         <f>'raw data'!S13</f>
-        <v>3.5799999999999998E-2</v>
+        <v>1.5100000000000001E-2</v>
       </c>
       <c r="X15" s="4">
         <f>'raw data'!T13</f>
-        <v>0.1241</v>
+        <v>5.2400000000000002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1502,41 +1506,41 @@
       </c>
       <c r="C16" s="3">
         <f>'raw data'!C14</f>
-        <v>0.75</v>
+        <v>0.27</v>
       </c>
       <c r="D16" s="3">
         <f>'raw data'!D14</f>
-        <v>0.79</v>
+        <v>0.43</v>
       </c>
       <c r="E16" s="3">
         <f>'raw data'!E14</f>
-        <v>0.65</v>
+        <v>0.02</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="3">
         <f>'raw data'!F14</f>
-        <v>-0.22</v>
+        <v>0.08</v>
       </c>
       <c r="H16" s="3">
         <f>'raw data'!G14</f>
-        <v>0.14000000000000001</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="I16" s="3">
         <f>'raw data'!H14</f>
-        <v>-0.08</v>
+        <v>-0.43</v>
       </c>
       <c r="J16" s="3">
         <f>'raw data'!I14</f>
-        <v>0.19</v>
+        <v>0.09</v>
       </c>
       <c r="K16" s="3">
         <f>'raw data'!J14</f>
-        <v>0.14000000000000001</v>
+        <v>-0.05</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="3">
         <f>'raw data'!K14</f>
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="N16" s="3" t="str">
         <f>'raw data'!L14</f>
@@ -1544,20 +1548,20 @@
       </c>
       <c r="O16" s="3">
         <f>'raw data'!M14</f>
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="P16" s="7"/>
       <c r="Q16" s="3">
         <f>'raw data'!N14</f>
-        <v>0.52</v>
+        <v>-0.5</v>
       </c>
       <c r="R16" s="3">
         <f>'raw data'!O14</f>
-        <v>0.22</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="S16" s="3">
         <f>'raw data'!P14</f>
-        <v>0.06</v>
+        <v>0.49</v>
       </c>
       <c r="T16" s="7"/>
       <c r="U16" s="12" t="s">
@@ -1565,15 +1569,15 @@
       </c>
       <c r="V16" s="8">
         <f>'raw data'!Q14</f>
-        <v>8.5099999999999995E-2</v>
+        <v>0.33239999999999997</v>
       </c>
       <c r="W16" s="4">
         <f>'raw data'!S14</f>
-        <v>3.8199999999999998E-2</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="X16" s="4">
         <f>'raw data'!T14</f>
-        <v>0.13239999999999999</v>
+        <v>4.4299999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1585,45 +1589,45 @@
       </c>
       <c r="C17" s="3">
         <f>'raw data'!C15</f>
-        <v>0.6</v>
+        <v>0.36</v>
       </c>
       <c r="D17" s="3">
         <f>'raw data'!D15</f>
-        <v>0.63</v>
+        <v>0.34</v>
       </c>
       <c r="E17" s="3">
         <f>'raw data'!E15</f>
-        <v>0.46</v>
+        <v>-0.12</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="3">
         <f>'raw data'!F15</f>
-        <v>0.13</v>
+        <v>0.05</v>
       </c>
       <c r="H17" s="3">
         <f>'raw data'!G15</f>
-        <v>0.38</v>
+        <v>-0.32</v>
       </c>
       <c r="I17" s="3">
         <f>'raw data'!H15</f>
-        <v>0.16</v>
+        <v>-0.33</v>
       </c>
       <c r="J17" s="3">
         <f>'raw data'!I15</f>
-        <v>0.51</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K17" s="3">
         <f>'raw data'!J15</f>
-        <v>0.28000000000000003</v>
+        <v>-0.12</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="3">
         <f>'raw data'!K15</f>
-        <v>0.87</v>
+        <v>0.8</v>
       </c>
       <c r="N17" s="3">
         <f>'raw data'!L15</f>
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="O17" s="3" t="str">
         <f>'raw data'!M15</f>
@@ -1632,15 +1636,15 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="3">
         <f>'raw data'!N15</f>
-        <v>0.65</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="R17" s="3">
         <f>'raw data'!O15</f>
-        <v>0.17</v>
+        <v>0.34</v>
       </c>
       <c r="S17" s="3">
         <f>'raw data'!P15</f>
-        <v>0.23</v>
+        <v>0.69</v>
       </c>
       <c r="T17" s="7"/>
       <c r="U17" s="10" t="s">
@@ -1648,15 +1652,15 @@
       </c>
       <c r="V17" s="8">
         <f>'raw data'!Q15</f>
-        <v>0.17100000000000001</v>
+        <v>0.3896</v>
       </c>
       <c r="W17" s="4">
         <f>'raw data'!S15</f>
-        <v>4.8800000000000003E-2</v>
+        <v>2.5700000000000001E-2</v>
       </c>
       <c r="X17" s="4">
         <f>'raw data'!T15</f>
-        <v>0.16900000000000001</v>
+        <v>8.8900000000000007E-2</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1694,20 +1698,20 @@
       </c>
       <c r="C19" s="3">
         <f>'raw data'!C16</f>
-        <v>0.66</v>
+        <v>-0.05</v>
       </c>
       <c r="D19" s="3">
         <f>'raw data'!D16</f>
-        <v>0.62</v>
+        <v>0.01</v>
       </c>
       <c r="E19" s="3">
         <f>'raw data'!E16</f>
-        <v>0.56000000000000005</v>
+        <v>0.24</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="3">
         <f>'raw data'!F16</f>
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="H19" s="3">
         <f>'raw data'!G16</f>
@@ -1715,28 +1719,28 @@
       </c>
       <c r="I19" s="3">
         <f>'raw data'!H16</f>
-        <v>0.36</v>
+        <v>0.48</v>
       </c>
       <c r="J19" s="3">
         <f>'raw data'!I16</f>
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
       <c r="K19" s="3">
         <f>'raw data'!J16</f>
-        <v>0.4</v>
+        <v>0.18</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="3">
         <f>'raw data'!K16</f>
-        <v>0.6</v>
+        <v>-0.72</v>
       </c>
       <c r="N19" s="3">
         <f>'raw data'!L16</f>
-        <v>0.52</v>
+        <v>-0.5</v>
       </c>
       <c r="O19" s="3">
         <f>'raw data'!M16</f>
-        <v>0.65</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="P19" s="7"/>
       <c r="Q19" s="3" t="str">
@@ -1745,11 +1749,11 @@
       </c>
       <c r="R19" s="3">
         <f>'raw data'!O16</f>
-        <v>0.14000000000000001</v>
+        <v>-0.08</v>
       </c>
       <c r="S19" s="3">
         <f>'raw data'!P16</f>
-        <v>0.1</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="T19" s="7"/>
       <c r="U19" s="10" t="s">
@@ -1757,15 +1761,15 @@
       </c>
       <c r="V19" s="8">
         <f>'raw data'!Q16</f>
-        <v>7.7200000000000005E-2</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="W19" s="4">
         <f>'raw data'!S16</f>
-        <v>4.7300000000000002E-2</v>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="X19" s="4">
         <f>'raw data'!T16</f>
-        <v>0.16370000000000001</v>
+        <v>7.1900000000000006E-2</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1777,54 +1781,54 @@
       </c>
       <c r="C20" s="3">
         <f>'raw data'!C17</f>
-        <v>0.21</v>
+        <v>0.48</v>
       </c>
       <c r="D20" s="3">
         <f>'raw data'!D17</f>
-        <v>0.18</v>
+        <v>0.37</v>
       </c>
       <c r="E20" s="3">
         <f>'raw data'!E17</f>
-        <v>0.24</v>
+        <v>0.37</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="3">
         <f>'raw data'!F17</f>
-        <v>-0.03</v>
+        <v>-0.38</v>
       </c>
       <c r="H20" s="3">
         <f>'raw data'!G17</f>
-        <v>0.01</v>
+        <v>-0.35</v>
       </c>
       <c r="I20" s="3">
         <f>'raw data'!H17</f>
-        <v>-0.21</v>
+        <v>-0.38</v>
       </c>
       <c r="J20" s="3">
         <f>'raw data'!I17</f>
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="K20" s="3">
         <f>'raw data'!J17</f>
-        <v>0.14000000000000001</v>
+        <v>-0.2</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="3">
         <f>'raw data'!K17</f>
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
       <c r="N20" s="3">
         <f>'raw data'!L17</f>
-        <v>0.22</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="O20" s="3">
         <f>'raw data'!M17</f>
-        <v>0.17</v>
+        <v>0.34</v>
       </c>
       <c r="P20" s="7"/>
       <c r="Q20" s="3">
         <f>'raw data'!N17</f>
-        <v>0.14000000000000001</v>
+        <v>-0.08</v>
       </c>
       <c r="R20" s="3" t="str">
         <f>'raw data'!O17</f>
@@ -1832,7 +1836,7 @@
       </c>
       <c r="S20" s="3">
         <f>'raw data'!P17</f>
-        <v>-0.01</v>
+        <v>0.04</v>
       </c>
       <c r="T20" s="7"/>
       <c r="U20" s="12" t="s">
@@ -1840,15 +1844,15 @@
       </c>
       <c r="V20" s="8">
         <f>'raw data'!Q17</f>
-        <v>0.16389999999999999</v>
+        <v>7.3300000000000004E-2</v>
       </c>
       <c r="W20" s="4">
         <f>'raw data'!S17</f>
-        <v>4.2299999999999997E-2</v>
+        <v>2.41E-2</v>
       </c>
       <c r="X20" s="4">
         <f>'raw data'!T17</f>
-        <v>0.14660000000000001</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1860,58 +1864,58 @@
       </c>
       <c r="C21" s="3">
         <f>'raw data'!C18</f>
-        <v>-0.35</v>
+        <v>0.16</v>
       </c>
       <c r="D21" s="3">
         <f>'raw data'!D18</f>
-        <v>-0.25</v>
+        <v>0.22</v>
       </c>
       <c r="E21" s="3">
         <f>'raw data'!E18</f>
-        <v>-0.36</v>
+        <v>-0.32</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="3">
         <f>'raw data'!F18</f>
-        <v>0.73</v>
+        <v>0.43</v>
       </c>
       <c r="H21" s="3">
         <f>'raw data'!G18</f>
-        <v>0.77</v>
+        <v>0.26</v>
       </c>
       <c r="I21" s="3">
         <f>'raw data'!H18</f>
-        <v>0.76</v>
+        <v>0.32</v>
       </c>
       <c r="J21" s="3">
         <f>'raw data'!I18</f>
-        <v>0.81</v>
+        <v>0.66</v>
       </c>
       <c r="K21" s="3">
         <f>'raw data'!J18</f>
-        <v>0.54</v>
+        <v>0.24</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="3">
         <f>'raw data'!K18</f>
-        <v>-7.0000000000000007E-2</v>
+        <v>0.36</v>
       </c>
       <c r="N21" s="3">
         <f>'raw data'!L18</f>
-        <v>0.06</v>
+        <v>0.49</v>
       </c>
       <c r="O21" s="3">
         <f>'raw data'!M18</f>
-        <v>0.23</v>
+        <v>0.69</v>
       </c>
       <c r="P21" s="7"/>
       <c r="Q21" s="3">
         <f>'raw data'!N18</f>
-        <v>0.1</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="R21" s="3">
         <f>'raw data'!O18</f>
-        <v>-0.01</v>
+        <v>0.04</v>
       </c>
       <c r="S21" s="3" t="str">
         <f>'raw data'!P18</f>
@@ -1923,14 +1927,1257 @@
       </c>
       <c r="V21" s="8">
         <f>'raw data'!Q18</f>
-        <v>0.12740000000000001</v>
+        <v>0.15129999999999999</v>
       </c>
       <c r="W21" s="4">
         <f>'raw data'!S18</f>
-        <v>5.79E-2</v>
+        <v>2.5499999999999998E-2</v>
       </c>
       <c r="X21" s="4">
         <f>'raw data'!T18</f>
+        <v>8.8499999999999995E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:X3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:T21">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="-1"/>
+        <cfvo type="num" val="1"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <color theme="5" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5:V7 V15:V17">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AA94ACCA-68F5-45B6-AB77-B8AA04A08545}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V8:V13">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F508EAF6-A822-42D9-98CC-FC73CD26018F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V19:V21">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{791B8C98-C563-4249-B72C-289726AC9D37}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X5:X7 X9:X13 X15:X17 W5:W21 X19:X21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AA94ACCA-68F5-45B6-AB77-B8AA04A08545}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>V5:V7 V15:V17</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F508EAF6-A822-42D9-98CC-FC73CD26018F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>V8:V13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{791B8C98-C563-4249-B72C-289726AC9D37}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>V19:V21</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C9:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="1.42578125" customWidth="1"/>
+    <col min="12" max="12" width="1.42578125" customWidth="1"/>
+    <col min="16" max="16" width="1.42578125" customWidth="1"/>
+    <col min="20" max="20" width="1.42578125" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+    </row>
+    <row r="4" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="9"/>
+      <c r="U4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>-0.22</v>
+      </c>
+      <c r="I5" s="3">
+        <v>-0.35</v>
+      </c>
+      <c r="J5" s="3">
+        <v>-0.17</v>
+      </c>
+      <c r="K5" s="3">
+        <v>-0.23</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="S5" s="3">
+        <v>-0.35</v>
+      </c>
+      <c r="T5" s="7"/>
+      <c r="U5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="V5" s="8">
+        <v>0.13689999999999999</v>
+      </c>
+      <c r="W5" s="4">
+        <v>3.15E-2</v>
+      </c>
+      <c r="X5" s="4">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="I6" s="3">
+        <v>-0.31</v>
+      </c>
+      <c r="J6" s="3">
+        <v>-0.12</v>
+      </c>
+      <c r="K6" s="3">
+        <v>-0.25</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="S6" s="3">
+        <v>-0.25</v>
+      </c>
+      <c r="T6" s="7"/>
+      <c r="U6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="8">
+        <v>0.13350000000000001</v>
+      </c>
+      <c r="W6" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="X6" s="4">
+        <v>0.13170000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="3">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-0.31</v>
+      </c>
+      <c r="I7" s="3">
+        <v>-0.42</v>
+      </c>
+      <c r="J7" s="3">
+        <v>-0.27</v>
+      </c>
+      <c r="K7" s="3">
+        <v>-0.37</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="S7" s="3">
+        <v>-0.36</v>
+      </c>
+      <c r="T7" s="7"/>
+      <c r="U7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7" s="8">
+        <v>0.18540000000000001</v>
+      </c>
+      <c r="W7" s="4">
+        <v>4.36E-2</v>
+      </c>
+      <c r="X7" s="4">
+        <v>0.15090000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+    </row>
+    <row r="9" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="3">
+        <v>-0.17</v>
+      </c>
+      <c r="N9" s="3">
+        <v>-0.22</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="R9" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="T9" s="7"/>
+      <c r="U9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="V9" s="8">
+        <v>8.6E-3</v>
+      </c>
+      <c r="W9" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="X9" s="4">
+        <v>1.04E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-0.22</v>
+      </c>
+      <c r="D10" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-0.31</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="R10" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="T10" s="7"/>
+      <c r="U10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="V10" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="W10" s="4">
+        <v>1.11E-2</v>
+      </c>
+      <c r="X10" s="4">
+        <v>3.8399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-0.35</v>
+      </c>
+      <c r="D11" s="3">
+        <v>-0.31</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-0.42</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="3">
+        <v>-0.09</v>
+      </c>
+      <c r="N11" s="3">
+        <v>-0.08</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="R11" s="3">
+        <v>-0.21</v>
+      </c>
+      <c r="S11" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="T11" s="7"/>
+      <c r="U11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="V11" s="8">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="W11" s="4">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="X11" s="4">
+        <v>0.1358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3">
+        <v>-0.17</v>
+      </c>
+      <c r="D12" s="3">
+        <v>-0.12</v>
+      </c>
+      <c r="E12" s="3">
+        <v>-0.27</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="R12" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="T12" s="7"/>
+      <c r="U12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="8">
+        <v>5.1700000000000003E-2</v>
+      </c>
+      <c r="W12" s="4">
+        <v>1.17E-2</v>
+      </c>
+      <c r="X12" s="4">
+        <v>4.0399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-0.23</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.25</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-0.37</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="R13" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="T13" s="7"/>
+      <c r="U13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="V13" s="8">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="W13" s="4">
+        <v>1.44E-2</v>
+      </c>
+      <c r="X13" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+    </row>
+    <row r="15" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="3">
+        <v>-0.17</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I15" s="3">
+        <v>-0.09</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="M15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="R15" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="S15" s="3">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="T15" s="7"/>
+      <c r="U15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V15" s="8">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="W15" s="4">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="X15" s="4">
+        <v>0.1241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="3">
+        <v>-0.22</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I16" s="3">
+        <v>-0.08</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="R16" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="T16" s="7"/>
+      <c r="U16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16" s="8">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="W16" s="4">
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="X16" s="4">
+        <v>0.13239999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="R17" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="S17" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="T17" s="7"/>
+      <c r="U17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="V17" s="8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="W17" s="4">
+        <v>4.8800000000000003E-2</v>
+      </c>
+      <c r="X17" s="4">
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="M19" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="T19" s="7"/>
+      <c r="U19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" s="8">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="W19" s="4">
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="X19" s="4">
+        <v>0.16370000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I20" s="3">
+        <v>-0.21</v>
+      </c>
+      <c r="J20" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="N20" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S20" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="T20" s="7"/>
+      <c r="U20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="V20" s="8">
+        <v>0.16389999999999999</v>
+      </c>
+      <c r="W20" s="4">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="X20" s="4">
+        <v>0.14660000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3">
+        <v>-0.35</v>
+      </c>
+      <c r="D21" s="3">
+        <v>-0.25</v>
+      </c>
+      <c r="E21" s="3">
+        <v>-0.36</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="3">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="R21" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T21" s="7"/>
+      <c r="U21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="V21" s="8">
+        <v>0.12740000000000001</v>
+      </c>
+      <c r="W21" s="4">
+        <v>5.79E-2</v>
+      </c>
+      <c r="X21" s="4">
         <v>0.20069999999999999</v>
       </c>
     </row>
@@ -2056,19 +3303,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection sqref="A1:T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -2168,55 +3415,55 @@
         <v>23</v>
       </c>
       <c r="D5" s="3">
-        <v>0.98</v>
+        <v>0.93</v>
       </c>
       <c r="E5" s="3">
-        <v>0.97</v>
+        <v>0.69</v>
       </c>
       <c r="F5" s="3">
-        <v>-0.5</v>
+        <v>-0.67</v>
       </c>
       <c r="G5" s="3">
-        <v>-0.22</v>
+        <v>-0.64</v>
       </c>
       <c r="H5" s="3">
-        <v>-0.35</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="I5" s="3">
-        <v>-0.17</v>
+        <v>-0.39</v>
       </c>
       <c r="J5" s="3">
-        <v>-0.23</v>
+        <v>-0.61</v>
       </c>
       <c r="K5" s="3">
-        <v>0.76</v>
+        <v>0.39</v>
       </c>
       <c r="L5" s="3">
-        <v>0.75</v>
+        <v>0.27</v>
       </c>
       <c r="M5" s="3">
-        <v>0.6</v>
+        <v>0.36</v>
       </c>
       <c r="N5" s="3">
-        <v>0.66</v>
+        <v>-0.05</v>
       </c>
       <c r="O5" s="3">
-        <v>0.21</v>
+        <v>0.48</v>
       </c>
       <c r="P5" s="3">
-        <v>-0.35</v>
+        <v>0.16</v>
       </c>
       <c r="Q5" s="4">
-        <v>0.13689999999999999</v>
+        <v>0.25240000000000001</v>
       </c>
       <c r="R5" s="4">
-        <v>8.3000000000000001E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="S5" s="4">
-        <v>3.15E-2</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="T5" s="4">
-        <v>0.109</v>
+        <v>5.04E-2</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="38.25" x14ac:dyDescent="0.2">
@@ -2227,58 +3474,58 @@
         <v>5</v>
       </c>
       <c r="C6" s="3">
-        <v>0.98</v>
+        <v>0.93</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="3">
-        <v>0.96</v>
+        <v>0.71</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.5</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="G6" s="3">
-        <v>-0.19</v>
+        <v>-0.59</v>
       </c>
       <c r="H6" s="3">
-        <v>-0.31</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="I6" s="3">
-        <v>-0.12</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="J6" s="3">
-        <v>-0.25</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="K6" s="3">
-        <v>0.76</v>
+        <v>0.46</v>
       </c>
       <c r="L6" s="3">
-        <v>0.79</v>
+        <v>0.43</v>
       </c>
       <c r="M6" s="3">
-        <v>0.63</v>
+        <v>0.34</v>
       </c>
       <c r="N6" s="3">
-        <v>0.62</v>
+        <v>0.01</v>
       </c>
       <c r="O6" s="3">
-        <v>0.18</v>
+        <v>0.37</v>
       </c>
       <c r="P6" s="3">
-        <v>-0.25</v>
+        <v>0.22</v>
       </c>
       <c r="Q6" s="4">
-        <v>0.13350000000000001</v>
+        <v>0.2233</v>
       </c>
       <c r="R6" s="4">
-        <v>9.4000000000000004E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="S6" s="4">
-        <v>3.7999999999999999E-2</v>
+        <v>1.3899999999999999E-2</v>
       </c>
       <c r="T6" s="4">
-        <v>0.13170000000000001</v>
+        <v>4.8099999999999997E-2</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="38.25" x14ac:dyDescent="0.2">
@@ -2289,58 +3536,58 @@
         <v>6</v>
       </c>
       <c r="C7" s="3">
-        <v>0.97</v>
+        <v>0.69</v>
       </c>
       <c r="D7" s="3">
-        <v>0.96</v>
+        <v>0.71</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="3">
-        <v>-0.56999999999999995</v>
+        <v>-0.71</v>
       </c>
       <c r="G7" s="3">
-        <v>-0.31</v>
+        <v>-0.65</v>
       </c>
       <c r="H7" s="3">
-        <v>-0.42</v>
+        <v>-0.63</v>
       </c>
       <c r="I7" s="3">
-        <v>-0.27</v>
+        <v>-0.54</v>
       </c>
       <c r="J7" s="3">
-        <v>-0.37</v>
+        <v>-0.78</v>
       </c>
       <c r="K7" s="3">
-        <v>0.64</v>
+        <v>-0.03</v>
       </c>
       <c r="L7" s="3">
-        <v>0.65</v>
+        <v>0.02</v>
       </c>
       <c r="M7" s="3">
-        <v>0.46</v>
+        <v>-0.12</v>
       </c>
       <c r="N7" s="3">
-        <v>0.56000000000000005</v>
+        <v>0.24</v>
       </c>
       <c r="O7" s="3">
-        <v>0.24</v>
+        <v>0.37</v>
       </c>
       <c r="P7" s="3">
-        <v>-0.36</v>
+        <v>-0.32</v>
       </c>
       <c r="Q7" s="4">
-        <v>0.18540000000000001</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="R7" s="4">
-        <v>1.04E-2</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="S7" s="4">
-        <v>4.36E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="T7" s="4">
-        <v>0.15090000000000001</v>
+        <v>5.5199999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
@@ -2351,58 +3598,58 @@
         <v>7</v>
       </c>
       <c r="C8" s="3">
-        <v>-0.5</v>
+        <v>-0.67</v>
       </c>
       <c r="D8" s="3">
-        <v>-0.5</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="E8" s="3">
-        <v>-0.56999999999999995</v>
+        <v>-0.71</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="3">
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="H8" s="3">
-        <v>0.84</v>
+        <v>0.63</v>
       </c>
       <c r="I8" s="3">
-        <v>0.87</v>
+        <v>0.7</v>
       </c>
       <c r="J8" s="3">
-        <v>0.68</v>
+        <v>0.79</v>
       </c>
       <c r="K8" s="3">
-        <v>-0.17</v>
+        <v>-0.09</v>
       </c>
       <c r="L8" s="3">
-        <v>-0.22</v>
+        <v>0.08</v>
       </c>
       <c r="M8" s="3">
-        <v>0.13</v>
+        <v>0.05</v>
       </c>
       <c r="N8" s="3">
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="O8" s="3">
-        <v>-0.03</v>
+        <v>-0.38</v>
       </c>
       <c r="P8" s="3">
-        <v>0.73</v>
+        <v>0.43</v>
       </c>
       <c r="Q8" s="4">
-        <v>8.6E-3</v>
+        <v>-2.0000000000000001E-4</v>
       </c>
       <c r="R8" s="4">
-        <v>5.9999999999999995E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="S8" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="T8" s="4">
-        <v>1.04E-2</v>
+        <v>5.5999999999999999E-3</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
@@ -2413,58 +3660,58 @@
         <v>8</v>
       </c>
       <c r="C9" s="3">
-        <v>-0.22</v>
+        <v>-0.64</v>
       </c>
       <c r="D9" s="3">
-        <v>-0.19</v>
+        <v>-0.59</v>
       </c>
       <c r="E9" s="3">
-        <v>-0.31</v>
+        <v>-0.65</v>
       </c>
       <c r="F9" s="3">
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="3">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="I9" s="3">
-        <v>0.93</v>
+        <v>0.72</v>
       </c>
       <c r="J9" s="3">
         <v>0.87</v>
       </c>
       <c r="K9" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.47</v>
       </c>
       <c r="L9" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="M9" s="3">
-        <v>0.38</v>
+        <v>-0.32</v>
       </c>
       <c r="N9" s="3">
         <v>0.49</v>
       </c>
       <c r="O9" s="3">
-        <v>0.01</v>
+        <v>-0.35</v>
       </c>
       <c r="P9" s="3">
-        <v>0.77</v>
+        <v>0.26</v>
       </c>
       <c r="Q9" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>2.1100000000000001E-2</v>
       </c>
       <c r="R9" s="4">
-        <v>2.0999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="S9" s="4">
-        <v>1.11E-2</v>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="T9" s="4">
-        <v>3.8399999999999997E-2</v>
+        <v>2.0299999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
@@ -2475,58 +3722,58 @@
         <v>9</v>
       </c>
       <c r="C10" s="3">
-        <v>-0.35</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="D10" s="3">
-        <v>-0.31</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="E10" s="3">
-        <v>-0.42</v>
+        <v>-0.63</v>
       </c>
       <c r="F10" s="3">
-        <v>0.84</v>
+        <v>0.63</v>
       </c>
       <c r="G10" s="3">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="3">
-        <v>0.85</v>
+        <v>0.69</v>
       </c>
       <c r="J10" s="3">
-        <v>0.78</v>
+        <v>0.69</v>
       </c>
       <c r="K10" s="3">
-        <v>-0.09</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="L10" s="3">
-        <v>-0.08</v>
+        <v>-0.43</v>
       </c>
       <c r="M10" s="3">
-        <v>0.16</v>
+        <v>-0.33</v>
       </c>
       <c r="N10" s="3">
-        <v>0.36</v>
+        <v>0.48</v>
       </c>
       <c r="O10" s="3">
-        <v>-0.21</v>
+        <v>-0.38</v>
       </c>
       <c r="P10" s="3">
-        <v>0.76</v>
+        <v>0.32</v>
       </c>
       <c r="Q10" s="4">
-        <v>1.8499999999999999E-2</v>
+        <v>5.1900000000000002E-2</v>
       </c>
       <c r="R10" s="4">
-        <v>8.0999999999999996E-3</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="S10" s="4">
-        <v>3.9199999999999999E-2</v>
+        <v>1.8200000000000001E-2</v>
       </c>
       <c r="T10" s="4">
-        <v>0.1358</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -2537,58 +3784,58 @@
         <v>10</v>
       </c>
       <c r="C11" s="3">
-        <v>-0.17</v>
+        <v>-0.39</v>
       </c>
       <c r="D11" s="3">
-        <v>-0.12</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="E11" s="3">
-        <v>-0.27</v>
+        <v>-0.54</v>
       </c>
       <c r="F11" s="3">
-        <v>0.87</v>
+        <v>0.7</v>
       </c>
       <c r="G11" s="3">
-        <v>0.93</v>
+        <v>0.72</v>
       </c>
       <c r="H11" s="3">
-        <v>0.85</v>
+        <v>0.69</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>23</v>
       </c>
       <c r="J11" s="3">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="K11" s="3">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N11" s="3">
         <v>0.2</v>
       </c>
-      <c r="L11" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="M11" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="N11" s="3">
-        <v>0.45</v>
-      </c>
       <c r="O11" s="3">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="P11" s="3">
-        <v>0.81</v>
+        <v>0.66</v>
       </c>
       <c r="Q11" s="4">
-        <v>5.1700000000000003E-2</v>
+        <v>1.89E-2</v>
       </c>
       <c r="R11" s="4">
-        <v>2.8E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="S11" s="4">
-        <v>1.17E-2</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="T11" s="4">
-        <v>4.0399999999999998E-2</v>
+        <v>2.24E-2</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
@@ -2599,58 +3846,58 @@
         <v>11</v>
       </c>
       <c r="C12" s="3">
-        <v>-0.23</v>
+        <v>-0.61</v>
       </c>
       <c r="D12" s="3">
-        <v>-0.25</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="E12" s="3">
-        <v>-0.37</v>
+        <v>-0.78</v>
       </c>
       <c r="F12" s="3">
-        <v>0.68</v>
+        <v>0.79</v>
       </c>
       <c r="G12" s="3">
         <v>0.87</v>
       </c>
       <c r="H12" s="3">
-        <v>0.78</v>
+        <v>0.69</v>
       </c>
       <c r="I12" s="3">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="3">
-        <v>0.21</v>
+        <v>-0.13</v>
       </c>
       <c r="L12" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.05</v>
       </c>
       <c r="M12" s="3">
-        <v>0.28000000000000003</v>
+        <v>-0.12</v>
       </c>
       <c r="N12" s="3">
-        <v>0.4</v>
+        <v>0.18</v>
       </c>
       <c r="O12" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.2</v>
       </c>
       <c r="P12" s="3">
-        <v>0.54</v>
+        <v>0.24</v>
       </c>
       <c r="Q12" s="4">
-        <v>8.9999999999999998E-4</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="R12" s="4">
-        <v>2E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="S12" s="4">
-        <v>1.44E-2</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="T12" s="4">
-        <v>0.05</v>
+        <v>2.5499999999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -2661,58 +3908,58 @@
         <v>12</v>
       </c>
       <c r="C13" s="3">
-        <v>0.76</v>
+        <v>0.39</v>
       </c>
       <c r="D13" s="3">
-        <v>0.76</v>
+        <v>0.46</v>
       </c>
       <c r="E13" s="3">
-        <v>0.64</v>
+        <v>-0.03</v>
       </c>
       <c r="F13" s="3">
-        <v>-0.17</v>
+        <v>-0.09</v>
       </c>
       <c r="G13" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.47</v>
       </c>
       <c r="H13" s="3">
-        <v>-0.09</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="I13" s="3">
-        <v>0.2</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="J13" s="3">
-        <v>0.21</v>
+        <v>-0.13</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="L13" s="3">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="M13" s="3">
-        <v>0.87</v>
+        <v>0.8</v>
       </c>
       <c r="N13" s="3">
-        <v>0.6</v>
+        <v>-0.72</v>
       </c>
       <c r="O13" s="3">
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
       <c r="P13" s="3">
-        <v>-7.0000000000000007E-2</v>
+        <v>0.36</v>
       </c>
       <c r="Q13" s="4">
-        <v>8.5099999999999995E-2</v>
+        <v>0.31669999999999998</v>
       </c>
       <c r="R13" s="4">
-        <v>1.11E-2</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="S13" s="4">
-        <v>3.5799999999999998E-2</v>
+        <v>1.5100000000000001E-2</v>
       </c>
       <c r="T13" s="4">
-        <v>0.1241</v>
+        <v>5.2400000000000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
@@ -2723,58 +3970,58 @@
         <v>13</v>
       </c>
       <c r="C14" s="3">
-        <v>0.75</v>
+        <v>0.27</v>
       </c>
       <c r="D14" s="3">
-        <v>0.79</v>
+        <v>0.43</v>
       </c>
       <c r="E14" s="3">
-        <v>0.65</v>
+        <v>0.02</v>
       </c>
       <c r="F14" s="3">
-        <v>-0.22</v>
+        <v>0.08</v>
       </c>
       <c r="G14" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="H14" s="3">
-        <v>-0.08</v>
+        <v>-0.43</v>
       </c>
       <c r="I14" s="3">
-        <v>0.19</v>
+        <v>0.09</v>
       </c>
       <c r="J14" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.05</v>
       </c>
       <c r="K14" s="3">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="M14" s="3">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="N14" s="3">
-        <v>0.52</v>
+        <v>-0.5</v>
       </c>
       <c r="O14" s="3">
-        <v>0.22</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="P14" s="3">
-        <v>0.06</v>
+        <v>0.49</v>
       </c>
       <c r="Q14" s="4">
-        <v>8.5099999999999995E-2</v>
+        <v>0.33239999999999997</v>
       </c>
       <c r="R14" s="4">
-        <v>1.03E-2</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="S14" s="4">
-        <v>3.8199999999999998E-2</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="T14" s="4">
-        <v>0.13239999999999999</v>
+        <v>4.4299999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
@@ -2785,58 +4032,58 @@
         <v>14</v>
       </c>
       <c r="C15" s="3">
-        <v>0.6</v>
+        <v>0.36</v>
       </c>
       <c r="D15" s="3">
-        <v>0.63</v>
+        <v>0.34</v>
       </c>
       <c r="E15" s="3">
-        <v>0.46</v>
+        <v>-0.12</v>
       </c>
       <c r="F15" s="3">
-        <v>0.13</v>
+        <v>0.05</v>
       </c>
       <c r="G15" s="3">
-        <v>0.38</v>
+        <v>-0.32</v>
       </c>
       <c r="H15" s="3">
-        <v>0.16</v>
+        <v>-0.33</v>
       </c>
       <c r="I15" s="3">
-        <v>0.51</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J15" s="3">
-        <v>0.28000000000000003</v>
+        <v>-0.12</v>
       </c>
       <c r="K15" s="3">
-        <v>0.87</v>
+        <v>0.8</v>
       </c>
       <c r="L15" s="3">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="N15" s="3">
-        <v>0.65</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="O15" s="3">
-        <v>0.17</v>
+        <v>0.34</v>
       </c>
       <c r="P15" s="3">
-        <v>0.23</v>
+        <v>0.69</v>
       </c>
       <c r="Q15" s="4">
-        <v>0.17100000000000001</v>
+        <v>0.3896</v>
       </c>
       <c r="R15" s="4">
-        <v>1.3100000000000001E-2</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="S15" s="4">
-        <v>4.8800000000000003E-2</v>
+        <v>2.5700000000000001E-2</v>
       </c>
       <c r="T15" s="4">
-        <v>0.16900000000000001</v>
+        <v>8.8900000000000007E-2</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -2847,58 +4094,58 @@
         <v>15</v>
       </c>
       <c r="C16" s="3">
-        <v>0.66</v>
+        <v>-0.05</v>
       </c>
       <c r="D16" s="3">
-        <v>0.62</v>
+        <v>0.01</v>
       </c>
       <c r="E16" s="3">
-        <v>0.56000000000000005</v>
+        <v>0.24</v>
       </c>
       <c r="F16" s="3">
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="G16" s="3">
         <v>0.49</v>
       </c>
       <c r="H16" s="3">
-        <v>0.36</v>
+        <v>0.48</v>
       </c>
       <c r="I16" s="3">
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
       <c r="J16" s="3">
-        <v>0.4</v>
+        <v>0.18</v>
       </c>
       <c r="K16" s="3">
-        <v>0.6</v>
+        <v>-0.72</v>
       </c>
       <c r="L16" s="3">
-        <v>0.52</v>
+        <v>-0.5</v>
       </c>
       <c r="M16" s="3">
-        <v>0.65</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="O16" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.08</v>
       </c>
       <c r="P16" s="3">
-        <v>0.1</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="Q16" s="4">
-        <v>7.7200000000000005E-2</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="R16" s="4">
-        <v>1.04E-2</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="S16" s="4">
-        <v>4.7300000000000002E-2</v>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="T16" s="4">
-        <v>0.16370000000000001</v>
+        <v>7.1900000000000006E-2</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
@@ -2909,58 +4156,58 @@
         <v>16</v>
       </c>
       <c r="C17" s="3">
-        <v>0.21</v>
+        <v>0.48</v>
       </c>
       <c r="D17" s="3">
-        <v>0.18</v>
+        <v>0.37</v>
       </c>
       <c r="E17" s="3">
-        <v>0.24</v>
+        <v>0.37</v>
       </c>
       <c r="F17" s="3">
-        <v>-0.03</v>
+        <v>-0.38</v>
       </c>
       <c r="G17" s="3">
-        <v>0.01</v>
+        <v>-0.35</v>
       </c>
       <c r="H17" s="3">
-        <v>-0.21</v>
+        <v>-0.38</v>
       </c>
       <c r="I17" s="3">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="J17" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="L17" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K17" s="3">
-        <v>0.24</v>
-      </c>
-      <c r="L17" s="3">
-        <v>0.22</v>
-      </c>
       <c r="M17" s="3">
-        <v>0.17</v>
+        <v>0.34</v>
       </c>
       <c r="N17" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.08</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="P17" s="3">
-        <v>-0.01</v>
+        <v>0.04</v>
       </c>
       <c r="Q17" s="4">
-        <v>0.16389999999999999</v>
+        <v>7.3300000000000004E-2</v>
       </c>
       <c r="R17" s="4">
-        <v>1.0999999999999999E-2</v>
+        <v>7.6E-3</v>
       </c>
       <c r="S17" s="4">
-        <v>4.2299999999999997E-2</v>
+        <v>2.41E-2</v>
       </c>
       <c r="T17" s="4">
-        <v>0.14660000000000001</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="38.25" x14ac:dyDescent="0.2">
@@ -2971,58 +4218,58 @@
         <v>17</v>
       </c>
       <c r="C18" s="3">
-        <v>-0.35</v>
+        <v>0.16</v>
       </c>
       <c r="D18" s="3">
-        <v>-0.25</v>
+        <v>0.22</v>
       </c>
       <c r="E18" s="3">
-        <v>-0.36</v>
+        <v>-0.32</v>
       </c>
       <c r="F18" s="3">
-        <v>0.73</v>
+        <v>0.43</v>
       </c>
       <c r="G18" s="3">
-        <v>0.77</v>
+        <v>0.26</v>
       </c>
       <c r="H18" s="3">
-        <v>0.76</v>
+        <v>0.32</v>
       </c>
       <c r="I18" s="3">
-        <v>0.81</v>
+        <v>0.66</v>
       </c>
       <c r="J18" s="3">
-        <v>0.54</v>
+        <v>0.24</v>
       </c>
       <c r="K18" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="N18" s="3">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="L18" s="3">
-        <v>0.06</v>
-      </c>
-      <c r="M18" s="3">
-        <v>0.23</v>
-      </c>
-      <c r="N18" s="3">
-        <v>0.1</v>
-      </c>
       <c r="O18" s="3">
-        <v>-0.01</v>
+        <v>0.04</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="Q18" s="4">
-        <v>0.12740000000000001</v>
+        <v>0.15129999999999999</v>
       </c>
       <c r="R18" s="4">
-        <v>0.01</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="S18" s="4">
-        <v>5.79E-2</v>
+        <v>2.5499999999999998E-2</v>
       </c>
       <c r="T18" s="4">
-        <v>0.20069999999999999</v>
+        <v>8.8499999999999995E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>